<commit_message>
msg auto mation needs to be ijmplemented
</commit_message>
<xml_diff>
--- a/FB_AGENCY_MESSAGE_INTRO.xlsx
+++ b/FB_AGENCY_MESSAGE_INTRO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PROFILE_LOCKSTATE</t>
   </si>
@@ -34,53 +34,14 @@
     <t>MESSAGE_INTRO_SCRIPT_FILL</t>
   </si>
   <si>
-    <t>OPEN</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/rips.gel</t>
-  </si>
-  <si>
-    <t>Zarin</t>
-  </si>
-  <si>
-    <t>Zara Khan</t>
-  </si>
-  <si>
-    <t>Shizuka</t>
-  </si>
-  <si>
-    <t>Hi NAME_FIRST what area in Dhaka are you?</t>
-  </si>
-  <si>
-    <t>Hi Zarin what area in Dhaka are you?</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/bushra.mithila</t>
-  </si>
-  <si>
-    <t>AUTOFILL</t>
-  </si>
-  <si>
-    <t>SCRIPT_1</t>
-  </si>
-  <si>
-    <t>FUNCTION(SCRIPT_1, NAME_FIRST)</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/noyona.orshi</t>
-  </si>
-  <si>
-    <t>SCRIPT_6</t>
-  </si>
-  <si>
-    <t>FUNCTION(SCRIPT_6, NAME_NICKNAME)</t>
+    <t>https://www.facebook.com/anm.sakib98</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -93,26 +54,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <u/>
       <sz val="11.0"/>
-      <color rgb="FF4472C4"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
       <sz val="11.0"/>
       <color rgb="FF4472C4"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11.0"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -199,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -218,40 +167,22 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -502,261 +433,225 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="10"/>
-      <c r="B3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="10"/>
-      <c r="B4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="10"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="10"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="16"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="10"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="16"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="10"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="16"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="10"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="16"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="10"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="16"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="10"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="16"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="10"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="10"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="16"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="16"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="10"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="16"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="10"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="16"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="10"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="16"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="16"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="10"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="16"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="10"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="16"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="8"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="10"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="16"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="8"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23">
-      <c r="A23" s="18"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24">
@@ -782,9 +677,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>